<commit_message>
Handle special chars in course name gracefully
</commit_message>
<xml_diff>
--- a/test_courses.xlsx
+++ b/test_courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u1344001\source\repos\Video-Sorter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59984A9D-C7AB-487E-99C3-6CE74694C5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15834FC-6E5A-4713-A103-11D8988E50D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7155" yWindow="4245" windowWidth="21585" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Class list" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>Room (cleaned)</t>
   </si>
   <si>
-    <t>Course1</t>
-  </si>
-  <si>
     <t>Course2</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>FINCH, LANCE (00161189); MORALES, MATTHEW (01344001)</t>
+  </si>
+  <si>
+    <t>Course1: The Sequel</t>
   </si>
 </sst>
 </file>
@@ -652,9 +652,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -692,7 +692,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -798,7 +798,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -940,7 +940,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,13 +998,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1013,13 +1013,13 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="2">
         <v>4603</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1027,13 +1027,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1042,13 +1042,13 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2">
         <v>5200</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -1056,13 +1056,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1071,13 +1071,13 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2">
         <v>2100</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>

</xml_diff>